<commit_message>
Added related to user data
</commit_message>
<xml_diff>
--- a/agents.xlsx
+++ b/agents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpasc\OneDrive\Desktop\autoss\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpasc\OneDrive\Desktop\AutoSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA073C5-AE95-4D1C-923B-80105501D419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836D7824-C31A-453E-BB00-97D42FC356E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="2580" windowWidth="28800" windowHeight="11295" tabRatio="410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -515,9 +515,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -714,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1090,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" t="s">
         <v>142</v>
       </c>
       <c r="B31" s="5" t="s">

</xml_diff>

<commit_message>
added tons of features
</commit_message>
<xml_diff>
--- a/agents.xlsx
+++ b/agents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpasc\OneDrive\Desktop\AutoSS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpasc\OneDrive\Desktop\AutoSS-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836D7824-C31A-453E-BB00-97D42FC356E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02FB743-C75F-44D6-8874-0624EF62A497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="2580" windowWidth="28800" windowHeight="11295" tabRatio="410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>https://www.boletinoficial.gob.ar/seccion/primera</t>
   </si>
   <si>
-    <t>https://www.bcra.gob.ar/SistemasFinancierosYdePagos/Buscador_por_tipo_y_fecha.asp</t>
-  </si>
-  <si>
     <t>https://www.bcentral.cl/web/banco-central/buscador?categoria=Normativas/Circulares</t>
   </si>
   <si>
@@ -375,92 +372,95 @@
     <t>0978</t>
   </si>
   <si>
+    <t>0924</t>
+  </si>
+  <si>
+    <t>0925</t>
+  </si>
+  <si>
+    <t>0926</t>
+  </si>
+  <si>
+    <t>0927</t>
+  </si>
+  <si>
+    <t>0928</t>
+  </si>
+  <si>
+    <t>0883</t>
+  </si>
+  <si>
+    <t>0884</t>
+  </si>
+  <si>
+    <t>0886</t>
+  </si>
+  <si>
+    <t>0058</t>
+  </si>
+  <si>
+    <t>0048</t>
+  </si>
+  <si>
+    <t>0071</t>
+  </si>
+  <si>
+    <t>0073</t>
+  </si>
+  <si>
+    <t>0077</t>
+  </si>
+  <si>
+    <t>0898</t>
+  </si>
+  <si>
+    <t>0900</t>
+  </si>
+  <si>
+    <t>0901</t>
+  </si>
+  <si>
+    <t>0113</t>
+  </si>
+  <si>
+    <t>0116</t>
+  </si>
+  <si>
+    <t>0171</t>
+  </si>
+  <si>
+    <t>https://www.legifrance.gouv.fr/</t>
+  </si>
+  <si>
+    <t>https://www.thetakeoverpanel.org.uk/</t>
+  </si>
+  <si>
+    <t>0084 to 0087</t>
+  </si>
+  <si>
+    <t>https://www.boe.es/diario_boe/ultimo.php</t>
+  </si>
+  <si>
+    <t>https://www.congress.gov/search?searchResultViewType=expanded&amp;pageSort=latestAction%3Adesc&amp;q=%7B%22congress%22%3A%5B%22118%22%5D%2C%22source%22%3A%22legislation%22%2C%22type%22%3A%22bills%22%2C%22bill-status%22%3A%22law%22%7D</t>
+  </si>
+  <si>
+    <t>0210_fedreg</t>
+  </si>
+  <si>
+    <t>https://gazette.gc.ca/rp-pr/p2/2024/index-eng.html</t>
+  </si>
+  <si>
+    <t>https://www.bcra.gob.ar/SistemasFinancierosYdePagos/Buscador_de_comunicaciones.asp</t>
+  </si>
+  <si>
     <t>0979</t>
-  </si>
-  <si>
-    <t>0924</t>
-  </si>
-  <si>
-    <t>0925</t>
-  </si>
-  <si>
-    <t>0926</t>
-  </si>
-  <si>
-    <t>0927</t>
-  </si>
-  <si>
-    <t>0928</t>
-  </si>
-  <si>
-    <t>0883</t>
-  </si>
-  <si>
-    <t>0884</t>
-  </si>
-  <si>
-    <t>0886</t>
-  </si>
-  <si>
-    <t>0058</t>
-  </si>
-  <si>
-    <t>0048</t>
-  </si>
-  <si>
-    <t>0071</t>
-  </si>
-  <si>
-    <t>0073</t>
-  </si>
-  <si>
-    <t>0077</t>
-  </si>
-  <si>
-    <t>0898</t>
-  </si>
-  <si>
-    <t>0900</t>
-  </si>
-  <si>
-    <t>0901</t>
-  </si>
-  <si>
-    <t>0113</t>
-  </si>
-  <si>
-    <t>0116</t>
-  </si>
-  <si>
-    <t>0171</t>
-  </si>
-  <si>
-    <t>https://www.legifrance.gouv.fr/</t>
-  </si>
-  <si>
-    <t>https://www.thetakeoverpanel.org.uk/</t>
-  </si>
-  <si>
-    <t>0084 to 0087</t>
-  </si>
-  <si>
-    <t>https://www.boe.es/diario_boe/ultimo.php</t>
-  </si>
-  <si>
-    <t>https://www.congress.gov/search?searchResultViewType=expanded&amp;pageSort=latestAction%3Adesc&amp;q=%7B%22congress%22%3A%5B%22118%22%5D%2C%22source%22%3A%22legislation%22%2C%22type%22%3A%22bills%22%2C%22bill-status%22%3A%22law%22%7D</t>
-  </si>
-  <si>
-    <t>0210_fedreg</t>
-  </si>
-  <si>
-    <t>https://gazette.gc.ca/rp-pr/p2/2024/index-eng.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,6 +473,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -492,12 +500,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -516,8 +527,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -712,7 +727,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,25 +753,25 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1140</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1140</v>
+      <c r="A2" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1140</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1140</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -764,13 +779,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -778,101 +793,101 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>8</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="B7" s="5" t="s">
-        <v>141</v>
+        <v>92</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1118</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1118</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1118</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1118</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>19</v>
@@ -880,13 +895,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>22</v>
@@ -894,13 +909,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>25</v>
@@ -911,68 +926,68 @@
         <v>23</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
       <c r="B20" s="5" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>32</v>
+      <c r="A21" t="s">
+        <v>29</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>34</v>
@@ -980,13 +995,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>37</v>
@@ -994,13 +1009,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>40</v>
@@ -1008,13 +1023,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>43</v>
@@ -1022,13 +1037,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>46</v>
@@ -1036,13 +1051,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1050,87 +1065,87 @@
         <v>47</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B29" s="5">
         <v>1139</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C29" s="5">
         <v>1139</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="5" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>142</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1138,208 +1153,208 @@
         <v>53</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B53" s="5">
         <v>1013</v>
@@ -1347,107 +1362,107 @@
       <c r="C53" s="5">
         <v>1013</v>
       </c>
+      <c r="D53" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="C54" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="C55" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="C58" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B62" s="5">
         <v>1130</v>
@@ -1458,89 +1473,92 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BC6D876A-2384-49F6-A95E-CD7063DDE930}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <ignoredErrors>
-    <ignoredError sqref="B5:B6 B16:B19 B8:B11 B26:B36 B39:B53 B56:B57 B59:B68" numberStoredAsText="1"/>
+    <ignoredError sqref="B6:B7 B17:B20 B9:B12 B27:B37 B40:B44 B56:B57 B59:B68 B45:B53" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>